<commit_message>
IMP:	- Column dimensions
</commit_message>
<xml_diff>
--- a/omnia_inventory_valuation/models/inventory_valuation.xlsx
+++ b/omnia_inventory_valuation/models/inventory_valuation.xlsx
@@ -455,7 +455,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" recordCount="2" createdVersion="3">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" recordCount="1" createdVersion="3">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F442" sheet="data_sheet"/>
   </cacheSource>
@@ -500,15 +500,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="2">
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="1">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -569,7 +561,7 @@
   <dimension ref="A1:F150091"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:F3"/>
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -645,12 +637,18 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="A3:F3 B9"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -694,13 +692,13 @@
         <v>6</v>
       </c>
       <c r="D3" s="16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -722,13 +720,13 @@
       <c r="B5" s="24"/>
       <c r="C5" s="25"/>
       <c r="D5" s="26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" s="27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>